<commit_message>
updates to figures for resubmission of 2019 synthesis paper
</commit_message>
<xml_diff>
--- a/data/2019 Cage Deployment Dates.xlsx
+++ b/data/2019 Cage Deployment Dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cawater-my.sharepoint.com/personal/rosemary_hartman_water_ca_gov/Documents/smelt cages/Smelt-cages/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{49946FF3-E417-4F6A-9C80-2292554D63A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{112AD378-D39D-4957-8561-B04EF34D8354}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="8_{49946FF3-E417-4F6A-9C80-2292554D63A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A092F69A-97C7-46D3-AED3-D67667F3191D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>Winter</t>
   </si>
   <si>
-    <t>SDWSC</t>
-  </si>
-  <si>
     <t>Summer</t>
   </si>
   <si>
@@ -66,6 +63,9 @@
   </si>
   <si>
     <t>StationID</t>
+  </si>
+  <si>
+    <t>DWS</t>
   </si>
 </sst>
 </file>
@@ -611,9 +611,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -651,7 +651,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -757,7 +757,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -899,7 +899,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -910,7 +910,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -924,7 +924,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -938,7 +938,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>43488</v>
@@ -952,7 +952,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>43523</v>
@@ -963,10 +963,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="1">
         <v>43676</v>
@@ -977,10 +977,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1">
         <v>43676</v>
@@ -991,10 +991,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
       </c>
       <c r="C6" s="1">
         <v>43747</v>
@@ -1005,10 +1005,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="1">
         <v>43747</v>
@@ -1019,10 +1019,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" s="1">
         <v>43747</v>

</xml_diff>